<commit_message>
Kommentare, Animationen, Gewinner Nachricht
</commit_message>
<xml_diff>
--- a/Quellen.xlsx
+++ b/Quellen.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$C$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$C$5</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -446,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +505,7 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -517,9 +517,10 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{506BB6A5-4AED-49BF-AC73-2F5BC0E548DA}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{4B00EEAD-412F-4483-BDB2-3B537AE36693}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{90276D57-0EF8-40BF-A93E-55444BB7531C}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{7ACBCEFC-10EB-4B89-A387-24F561305056}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="69" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="69" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>